<commit_message>
Update Gradebook and README; add relative reference example files
</commit_message>
<xml_diff>
--- a/Gradebook.xlsx
+++ b/Gradebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gurma\Documents\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gurma\Documents\ExcelProjects-101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA80BC2B-E80D-4DDC-B6CD-12FBB87A9302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1739D1B0-F9E0-4A0E-A1EA-AA078D9ACF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D12FA68F-C55E-4A1B-B861-18A95741F88D}"/>
   </bookViews>
@@ -270,7 +270,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="136">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -300,941 +300,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1280,331 +350,36 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="1"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2017,6 +792,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2024,7 +800,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2452,6 +1227,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2459,7 +1235,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2886,6 +1661,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2893,7 +1669,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4597,16 +3372,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>314324</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>561973</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>158522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>84364</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4634,15 +3409,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>147638</xdr:rowOff>
+      <xdr:colOff>340178</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>128588</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4989,8 +3764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB4CCDC-159A-4B37-8496-D35992CAAAA8}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5086,7 +3861,7 @@
         <v>0.7</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:L19" si="0">D4/D$2</f>
+        <f t="shared" ref="I4:K19" si="0">D4/D$2</f>
         <v>0.56666666666666665</v>
       </c>
       <c r="J4" s="2">
@@ -6203,6 +4978,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C28">
+    <cfRule type="iconSet" priority="17">
+      <iconSet iconSet="4TrafficLights">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="25"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="percent" val="75"/>
+      </iconSet>
+    </cfRule>
     <cfRule type="iconSet" priority="22">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -6210,7 +4993,19 @@
         <cfvo type="percent" val="67"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="17">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D28">
+    <cfRule type="iconSet" priority="18">
+      <iconSet iconSet="4TrafficLights">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="25"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="percent" val="75"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E28">
+    <cfRule type="iconSet" priority="19">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -6229,77 +5024,47 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E28">
-    <cfRule type="iconSet" priority="19">
-      <iconSet iconSet="4TrafficLights">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="25"/>
-        <cfvo type="percent" val="50"/>
-        <cfvo type="percent" val="75"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D28">
-    <cfRule type="iconSet" priority="18">
-      <iconSet iconSet="4TrafficLights">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="25"/>
-        <cfvo type="percent" val="50"/>
-        <cfvo type="percent" val="75"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H4:K28 M4:M28">
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="15" operator="lessThan">
-      <formula>30</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="lessThan">
-      <formula>0.3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="lessThan">
-      <formula>0.3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="lessThan">
-      <formula>0.3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="lessThan">
-      <formula>0.3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="greaterThan">
-      <formula>0.7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="lessThan">
+      <formula>30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M28 H4:K28">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
-      <formula>0.5</formula>
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
+      <formula>0.7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="lessThan">
+      <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M28">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>